<commit_message>
logs logs and more logs
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="183">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -657,13 +657,31 @@
     <t xml:space="preserve">   a) correct sponsoring behavior</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log2.txt(39-53, 117, 118)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log2.txt(39-53, 117, 118), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log1.txt(40-53)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">   b) correct behavior for quest participation</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log2.txt(57-63, 70-75, 101-104)</t>
+    <t xml:space="preserve">ai_strategy2_log2.txt(57-63, 70-75, 101-104), ai_strategy2_battleEquip_log4.txt(66-78)</t>
   </si>
   <si>
     <t xml:space="preserve">   c) correct behavior for tournaments</t>
@@ -672,7 +690,25 @@
     <t xml:space="preserve">   d) correct behavior for bidding</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log2.txt(86-97)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log1.txt(94-109), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log2.txt(86-97), ai_strategy2_log3.txt(111-115)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">is the rule of increasing BPs enforced</t>
@@ -759,7 +795,13 @@
     <t xml:space="preserve">lancelot</t>
   </si>
   <si>
+    <t xml:space="preserve">ai_strategy2_log2.txt(76, 81, 111[Battle points w/ Sir Lancelot])</t>
+  </si>
+  <si>
     <t xml:space="preserve">galahad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ai_strategy2_battleEquip_log4.txt(75, 77, 84)</t>
   </si>
   <si>
     <t xml:space="preserve">merlin</t>
@@ -982,7 +1024,7 @@
   <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
+      <selection pane="topLeft" activeCell="D89" activeCellId="0" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1172,7 +1214,7 @@
       <c r="C23" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1216,7 +1258,7 @@
       <c r="C32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1230,7 +1272,7 @@
       <c r="C33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1244,7 +1286,7 @@
       <c r="C34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1258,7 +1300,7 @@
       <c r="C35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1272,7 +1314,7 @@
       <c r="C36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1286,7 +1328,7 @@
       <c r="C37" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1300,7 +1342,7 @@
       <c r="C38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1319,7 +1361,7 @@
       <c r="C40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1338,7 +1380,7 @@
       <c r="C42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1352,7 +1394,7 @@
       <c r="C43" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1366,7 +1408,7 @@
       <c r="C44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1380,7 +1422,7 @@
       <c r="C45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1394,7 +1436,7 @@
       <c r="C46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1408,7 +1450,7 @@
       <c r="C47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1422,7 +1464,7 @@
       <c r="C48" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1441,7 +1483,7 @@
       <c r="C50" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1455,7 +1497,7 @@
       <c r="C51" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1469,7 +1511,7 @@
       <c r="C52" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1483,7 +1525,7 @@
       <c r="C53" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1497,7 +1539,7 @@
       <c r="C54" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1511,7 +1553,7 @@
       <c r="C55" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1525,7 +1567,7 @@
       <c r="C56" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1539,7 +1581,7 @@
       <c r="C57" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1553,7 +1595,7 @@
       <c r="C58" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1572,7 +1614,7 @@
       <c r="C60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1586,7 +1628,7 @@
       <c r="C61" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1600,7 +1642,7 @@
       <c r="C62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1614,7 +1656,7 @@
       <c r="C63" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1628,7 +1670,7 @@
       <c r="C64" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1652,7 +1694,7 @@
       <c r="C69" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1666,7 +1708,7 @@
       <c r="C70" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="5" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1680,7 +1722,7 @@
       <c r="C71" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1713,7 +1755,7 @@
       <c r="C75" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1724,7 +1766,7 @@
       <c r="C76" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1738,7 +1780,7 @@
       <c r="C77" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="5" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1757,7 +1799,7 @@
       <c r="C79" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1771,7 +1813,7 @@
       <c r="C80" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1785,7 +1827,7 @@
       <c r="C81" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="5" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1799,7 +1841,7 @@
       <c r="C82" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="5" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1813,7 +1855,7 @@
       <c r="C83" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1834,7 +1876,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>123</v>
       </c>
@@ -1858,7 +1900,7 @@
       <c r="C89" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="5" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1871,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>128</v>
       </c>
@@ -1937,7 +1979,7 @@
       <c r="C95" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="5" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1984,7 +2026,9 @@
       <c r="A99" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B99" s="6"/>
+      <c r="B99" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
       </c>
@@ -2030,7 +2074,7 @@
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D103" s="5" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2099,19 +2143,25 @@
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D110" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="D111" s="0" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
@@ -2120,7 +2170,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2129,7 +2179,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
@@ -2138,7 +2188,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
@@ -2147,7 +2197,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
@@ -2156,7 +2206,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
@@ -2165,7 +2215,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
@@ -2174,7 +2224,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
@@ -2183,7 +2233,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2192,12 +2242,12 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B122" s="6"/>
       <c r="C122" s="0" t="n">
@@ -2206,7 +2256,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B123" s="6"/>
       <c r="C123" s="0" t="n">
@@ -2215,7 +2265,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B124" s="6"/>
       <c r="C124" s="0" t="n">
@@ -2224,7 +2274,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B125" s="6"/>
       <c r="C125" s="0" t="n">
@@ -2233,7 +2283,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B126" s="6"/>
       <c r="C126" s="0" t="n">
@@ -2242,7 +2292,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B127" s="6"/>
       <c r="C127" s="0" t="n">
@@ -2251,7 +2301,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2260,12 +2310,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2276,7 +2326,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2287,7 +2337,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2296,7 +2346,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to redo logs - event prosperity log came from ai controller
also event queens favor and court called to camelot
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="187">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -678,7 +678,7 @@
     <t xml:space="preserve">is the rule of increasing BPs enforced</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(12)</t>
+    <t xml:space="preserve">scenario3.txt(12), event_log1.txt(41)</t>
   </si>
   <si>
     <t xml:space="preserve">is the rule of a max of 12 cards enforced?</t>
@@ -690,16 +690,19 @@
     <t xml:space="preserve">is the rule of no repeated weapon enforced</t>
   </si>
   <si>
+    <t xml:space="preserve">scenario1.txt(39), scenario2.txt(21), event_log1.txt(137)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">does the UI help enforcing the rule of no repeated weapon</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenario1.txt(39), scenario2.txt(21)</t>
   </si>
   <si>
-    <t xml:space="preserve">does the UI help enforcing the rule of no repeated weapon</t>
-  </si>
-  <si>
     <t xml:space="preserve">is it possible for a participant to NOT play a card for a stage</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(62)</t>
+    <t xml:space="preserve">scenario1.txt(62), event_log1.txt(60)</t>
   </si>
   <si>
     <t xml:space="preserve">as the game starts, can I select 1 to 3 AI players? (as opposed to always the same # of AIs)</t>
@@ -986,8 +989,8 @@
   </sheetPr>
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D96" activeCellId="0" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1943,12 +1946,12 @@
         <v>0.5</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>21</v>
@@ -1957,12 +1960,12 @@
         <v>0.5</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>21</v>
@@ -1971,12 +1974,12 @@
         <v>0.5</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>21</v>
@@ -1987,7 +1990,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B99" s="6" t="n">
         <v>0</v>
@@ -1998,19 +2001,19 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="n">
@@ -2019,31 +2022,31 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
@@ -2052,7 +2055,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
@@ -2061,7 +2064,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
@@ -2070,7 +2073,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
@@ -2079,7 +2082,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
@@ -2088,43 +2091,43 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
@@ -2133,7 +2136,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2142,43 +2145,43 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
@@ -2187,7 +2190,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
@@ -2196,7 +2199,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
@@ -2205,7 +2208,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2214,12 +2217,12 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B122" s="6"/>
       <c r="C122" s="0" t="n">
@@ -2228,7 +2231,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B123" s="6"/>
       <c r="C123" s="0" t="n">
@@ -2237,7 +2240,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B124" s="6"/>
       <c r="C124" s="0" t="n">
@@ -2246,7 +2249,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B125" s="6"/>
       <c r="C125" s="0" t="n">
@@ -2255,7 +2258,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B126" s="6"/>
       <c r="C126" s="0" t="n">
@@ -2264,7 +2267,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B127" s="6"/>
       <c r="C127" s="0" t="n">
@@ -2273,7 +2276,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2282,12 +2285,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2298,7 +2301,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2309,7 +2312,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kings call to arms
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -717,6 +717,9 @@
     <t xml:space="preserve">do you support a 2-player game</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">test of morgan le fey</t>
   </si>
   <si>
@@ -726,6 +729,9 @@
     <t xml:space="preserve">test of the questing beast</t>
   </si>
   <si>
+    <t xml:space="preserve">event_log4.txt(64-94)</t>
+  </si>
+  <si>
     <t xml:space="preserve">amour</t>
   </si>
   <si>
@@ -798,10 +804,13 @@
     <t xml:space="preserve">king's call to arms</t>
   </si>
   <si>
+    <t xml:space="preserve">event_log3.txt(87-98), event_log4.txt(29-46, 108-119)</t>
+  </si>
+  <si>
     <t xml:space="preserve">queen's favor</t>
   </si>
   <si>
-    <t xml:space="preserve">event_log2(28-44)</t>
+    <t xml:space="preserve">event_log2(28-44), event_log3.txt(100-114)</t>
   </si>
   <si>
     <t xml:space="preserve">court called to camelot</t>
@@ -996,7 +1005,7 @@
   <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
+      <selection pane="topLeft" activeCell="C104" activeCellId="0" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1998,8 +2007,8 @@
       <c r="A99" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B99" s="6" t="n">
-        <v>0</v>
+      <c r="B99" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -2007,52 +2016,55 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="D101" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
@@ -2061,7 +2073,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
@@ -2070,7 +2082,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
@@ -2079,7 +2091,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
@@ -2088,7 +2100,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
@@ -2097,43 +2109,43 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
@@ -2142,7 +2154,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2151,76 +2163,79 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D117" s="0" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2229,66 +2244,78 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B122" s="6"/>
+        <v>180</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C122" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B123" s="6"/>
+        <v>181</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C123" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B124" s="6"/>
+        <v>182</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C124" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B125" s="6"/>
+        <v>183</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C125" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B126" s="6"/>
+        <v>184</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C126" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B127" s="6"/>
+        <v>185</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C127" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2297,12 +2324,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2313,7 +2340,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2324,7 +2351,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2333,7 +2360,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strategy2 tournament + log
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -712,6 +712,9 @@
   </si>
   <si>
     <t xml:space="preserve">are discarded cards reusable when A and/or S decks run out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ai_strategy2_log5.txt(50-68)</t>
   </si>
   <si>
     <t xml:space="preserve">do you support a 2-player game</t>
@@ -1004,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C104" activeCellId="0" sqref="C104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2002,13 +2005,16 @@
       <c r="C98" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="D98" s="0" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -2016,55 +2022,55 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
@@ -2073,7 +2079,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
@@ -2082,7 +2088,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
@@ -2091,7 +2097,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
@@ -2100,7 +2106,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
@@ -2109,43 +2115,43 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
@@ -2154,7 +2160,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2163,79 +2169,79 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2244,15 +2250,15 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>2</v>
@@ -2260,10 +2266,10 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>1</v>
@@ -2271,10 +2277,10 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>2</v>
@@ -2282,10 +2288,10 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>2</v>
@@ -2293,10 +2299,10 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>2</v>
@@ -2304,10 +2310,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>2</v>
@@ -2315,7 +2321,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2324,12 +2330,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2340,7 +2346,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2351,7 +2357,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2360,7 +2366,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deck proof log - reshuffle
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="194">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -669,6 +669,9 @@
     <t xml:space="preserve">   c) correct behavior for tournaments</t>
   </si>
   <si>
+    <t xml:space="preserve">ai_strategy2_log5.txt(50-68)</t>
+  </si>
+  <si>
     <t xml:space="preserve">   d) correct behavior for bidding</t>
   </si>
   <si>
@@ -714,7 +717,7 @@
     <t xml:space="preserve">are discarded cards reusable when A and/or S decks run out</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log5.txt(50-68)</t>
+    <t xml:space="preserve">deck_proof_log.txt(144-172, 586-617)</t>
   </si>
   <si>
     <t xml:space="preserve">do you support a 2-player game</t>
@@ -871,7 +874,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -909,6 +912,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -959,7 +968,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -988,6 +997,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1007,7 +1020,7 @@
   </sheetPr>
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
     </sheetView>
   </sheetViews>
@@ -1896,10 +1909,13 @@
       <c r="C90" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D90" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>21</v>
@@ -1908,12 +1924,12 @@
         <v>1</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>21</v>
@@ -1922,12 +1938,12 @@
         <v>0.5</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>21</v>
@@ -1936,12 +1952,12 @@
         <v>0.5</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>21</v>
@@ -1950,12 +1966,12 @@
         <v>0.5</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>21</v>
@@ -1964,12 +1980,12 @@
         <v>0.5</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>21</v>
@@ -1978,12 +1994,12 @@
         <v>0.5</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>21</v>
@@ -1992,12 +2008,12 @@
         <v>0.5</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>21</v>
@@ -2006,15 +2022,15 @@
         <v>0.5</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -2022,55 +2038,55 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
@@ -2079,7 +2095,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
@@ -2088,7 +2104,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
@@ -2097,7 +2113,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
@@ -2106,7 +2122,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
@@ -2115,43 +2131,43 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
@@ -2160,7 +2176,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2169,79 +2185,79 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2250,15 +2266,15 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>2</v>
@@ -2266,10 +2282,10 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>1</v>
@@ -2277,10 +2293,10 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>2</v>
@@ -2288,10 +2304,10 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>2</v>
@@ -2299,10 +2315,10 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>2</v>
@@ -2310,10 +2326,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>2</v>
@@ -2321,7 +2337,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2330,12 +2346,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2346,7 +2362,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2357,7 +2373,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2366,7 +2382,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up json / spring logging features
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -859,6 +859,9 @@
   </si>
   <si>
     <t xml:space="preserve">use of JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipment_info / quest_setup_cards</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -874,7 +877,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -912,12 +915,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -968,7 +965,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -997,10 +994,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1020,8 +1013,8 @@
   </sheetPr>
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D131" activeCellId="0" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1909,7 +1902,7 @@
       <c r="C90" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2370,10 +2363,13 @@
       <c r="C131" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D131" s="0" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2382,7 +2378,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re do of sceneario 1 2 3 log
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="197">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(9-23)</t>
+    <t xml:space="preserve">scenario1.txt(46-60)</t>
   </si>
   <si>
     <r>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">does each client open a GUI that shows the cards of this players as well as info of other players</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(24-27, 31)</t>
+    <t xml:space="preserve">scenario1.txt(61-65)</t>
   </si>
   <si>
     <t xml:space="preserve">  (for other players, must see rank, # of shields, # of cards)</t>
@@ -234,31 +234,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(28, 29)</t>
+    <t xml:space="preserve">scenario1.txt(67, 68)</t>
   </si>
   <si>
     <t xml:space="preserve">is only the GUI of player1 updated to offer accepting/declining this quest</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(30)</t>
+    <t xml:space="preserve">scenario1.txt(69)</t>
   </si>
   <si>
     <t xml:space="preserve">once player1 accepts sponsoring, are other players informed</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(34-37)</t>
+    <t xml:space="preserve">scenario1.txt(70-73)</t>
   </si>
   <si>
     <t xml:space="preserve">is only the GUI of p1 updated to allow him to select cards for BOTH stages</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(38)</t>
+    <t xml:space="preserve">scenario1.txt(74)</t>
   </si>
   <si>
     <t xml:space="preserve">is p1 able to select cards for BOTH  stages</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(40)</t>
+    <t xml:space="preserve">scenario1.txt(77)</t>
   </si>
   <si>
     <r>
@@ -294,13 +294,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(45)</t>
+    <t xml:space="preserve">scenario1.txt(82)</t>
   </si>
   <si>
     <t xml:space="preserve">once p2 accepts and gets an adventure card, is its GUI correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(46-48)</t>
+    <t xml:space="preserve">scenario1.txt(87-89)</t>
   </si>
   <si>
     <t xml:space="preserve">  (i.e., p2 sees the new adventure card)</t>
@@ -309,7 +309,7 @@
     <t xml:space="preserve">then, are the GUIs of p1, p3 and p4 correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(49)</t>
+    <t xml:space="preserve">scenario1.txt(90)</t>
   </si>
   <si>
     <t xml:space="preserve">   (that is, p1, p3 and p4 are informed p2 accepts AND see p2's # of cards increase by 1)</t>
@@ -318,37 +318,37 @@
     <t xml:space="preserve">then (and only then) does the GUI of p3 (and no other) asks if p3 participates</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(50)</t>
+    <t xml:space="preserve">scenario1.txt(91)</t>
   </si>
   <si>
     <t xml:space="preserve">once p3 accepts and gets an adventure card, is its GUI correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(51-53)</t>
+    <t xml:space="preserve">scenario1.txt(92-94)</t>
   </si>
   <si>
     <t xml:space="preserve">then, are the GUIs of p1, p2 and p4 correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(54)</t>
+    <t xml:space="preserve">scenario1.txt(95)</t>
   </si>
   <si>
     <t xml:space="preserve">then (and only then) does the GUI of p4 (and no other) asks if p4 participates</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(55)</t>
+    <t xml:space="preserve">scenario1.txt(96)</t>
   </si>
   <si>
     <t xml:space="preserve">once p4 accepts and gets an adventure card, is its GUI correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(56-58)</t>
+    <t xml:space="preserve">scenario1.txt(97-99)</t>
   </si>
   <si>
     <t xml:space="preserve">then, are the GUIs of p1, p2 and p3 correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(59)</t>
+    <t xml:space="preserve">scenario1.txt(100)</t>
   </si>
   <si>
     <r>
@@ -384,7 +384,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(60)</t>
+    <t xml:space="preserve">scenario1.txt(101)</t>
   </si>
   <si>
     <t xml:space="preserve">once p2, p3 and p4 have selected their cards for stage 1:</t>
@@ -396,19 +396,19 @@
     <t xml:space="preserve">    b) does the resolution of this stage show all the cards played by each participant to all players</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(61-67)</t>
+    <t xml:space="preserve">scenario1.txt(102-111)</t>
   </si>
   <si>
     <t xml:space="preserve">    c) does the resolution of this stage show to all players which ones are eliminated (here p2)</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(69-79, 74)</t>
+    <t xml:space="preserve">scenario1.txt(113-123, 118)</t>
   </si>
   <si>
     <t xml:space="preserve">    d) does the GUI of each player get updated by discarding the cards played for that stage</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(68)</t>
+    <t xml:space="preserve">scenario1.txt(112)</t>
   </si>
   <si>
     <t xml:space="preserve">    e) is the GUI of every other player updated to reflect the new number of cards of each player</t>
@@ -417,25 +417,25 @@
     <t xml:space="preserve">p2 is eliminated, p3  and p4 get a new adventure card shown in their GUI</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(81, 82)</t>
+    <t xml:space="preserve">scenario1.txt(127, 128)</t>
   </si>
   <si>
     <t xml:space="preserve">does the GUI of p3 (and the one of p4) prompt them to discard a card (not seen by others)</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(83)</t>
+    <t xml:space="preserve">scenario1.txt(129)</t>
   </si>
   <si>
     <t xml:space="preserve">is the GUI of p1 and of p2 updated to reflect the current # of cards of p3 and p4</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(84)</t>
+    <t xml:space="preserve">scenario1.txt(130)</t>
   </si>
   <si>
     <t xml:space="preserve">do their GUIs allow p3 and p4 select their cards for stage 2</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(85-89)</t>
+    <t xml:space="preserve">scenario1.txt(132-137)</t>
   </si>
   <si>
     <t xml:space="preserve">once this second stage is resolved</t>
@@ -444,13 +444,13 @@
     <t xml:space="preserve">  a) does the winner get the correct number of shields</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(95, 101)</t>
+    <t xml:space="preserve">scenario1.txt(143)</t>
   </si>
   <si>
     <t xml:space="preserve">  b) does the sponsor get the correct number of cards</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(102, 103)</t>
+    <t xml:space="preserve">scenario1.txt(145, 146)</t>
   </si>
   <si>
     <r>
@@ -486,19 +486,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(104)</t>
+    <t xml:space="preserve">scenario1.txt(149)</t>
   </si>
   <si>
     <t xml:space="preserve">next story card is "Chivalrous Deed": all GUIs are updated correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(107-118)</t>
+    <t xml:space="preserve">scenario1.txt(150-162)</t>
   </si>
   <si>
     <t xml:space="preserve">next story card is  “Prosperity throughout the kingdom”: all GUIs are updated correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(119-136)</t>
+    <t xml:space="preserve">scenario1.txt(163-181)</t>
   </si>
   <si>
     <r>
@@ -530,19 +530,19 @@
     <t xml:space="preserve">have p1, p2 and p4 participate: is this reflected in everyone's GUI (with p3 not participating)</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario2.txt(1-14, 20)</t>
+    <t xml:space="preserve">scenario2.txt(4-17, 23)</t>
   </si>
   <si>
     <t xml:space="preserve">is it possible for all participants to select their cards to play concurrently</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario2.txt(15-19)</t>
+    <t xml:space="preserve">scenario2.txt(18-22, 40-43)</t>
   </si>
   <si>
     <t xml:space="preserve">is resolution of tournament correctly handled in the GUI of each player</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario2.txt(22-57, 31, 51)</t>
+    <t xml:space="preserve">scenario2.txt(33-37, 49-54)</t>
   </si>
   <si>
     <r>
@@ -571,25 +571,25 @@
     <t xml:space="preserve">next story card is "Slay the dragon": all GUIs are correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(1, 2)</t>
+    <t xml:space="preserve">scenario3.txt(4, 5)</t>
   </si>
   <si>
     <t xml:space="preserve">the player who drew this quest declines: all GUIs are correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(3-5)</t>
+    <t xml:space="preserve">scenario3.txt(7-9)</t>
   </si>
   <si>
     <t xml:space="preserve">     next player sponsors and sets up the quest to have a test at the first stage</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(6-13)</t>
+    <t xml:space="preserve">scenario3.txt(10-20)</t>
   </si>
   <si>
     <t xml:space="preserve">     all other players participate and get an adventure card: all GUIs are correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(17-31)</t>
+    <t xml:space="preserve">scenario3.txt(21-37)</t>
   </si>
   <si>
     <t xml:space="preserve">     each participant bids IN TURN, but the first one bids a second time and wins the test</t>
@@ -598,31 +598,31 @@
     <t xml:space="preserve">            a) each bid is correctly broadcasted to sponsor and other participants</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(32-40)</t>
+    <t xml:space="preserve">scenario3.txt(38-49)</t>
   </si>
   <si>
     <t xml:space="preserve">            b) the winner is correctly determined and broadcast to all players</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(47, 48)</t>
+    <t xml:space="preserve">scenario3.txt(59, 60)</t>
   </si>
   <si>
     <t xml:space="preserve">            c) the winner discards the bidded # of cards: all GUIs are correctly updated</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(43-46) [only 2 discards – King Arthur +2 bids]</t>
+    <t xml:space="preserve">scenario3.txt(48, 4-56, 58) [only 3 discards out of 5 bids – King Arthur +2 bids]</t>
   </si>
   <si>
     <t xml:space="preserve">            d) two other participants are eliminated and do NOT get to the 2nd stage</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(41, 42)</t>
+    <t xml:space="preserve">scenario3.txt(50-53)</t>
   </si>
   <si>
     <t xml:space="preserve">            e) winner plays second stage but loses: this outcome is broadcasted to all</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(49-59, 57)</t>
+    <t xml:space="preserve">scenario3.txt(62-74, 70)</t>
   </si>
   <si>
     <t xml:space="preserve">Other functionality</t>
@@ -768,7 +768,7 @@
     <t xml:space="preserve">arthur</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario3.txt(39-44, 47) [player only discards 2 due to bonus bids]</t>
+    <t xml:space="preserve">scenario3.txt(48-56) [player only discards 3 due to bonus bids]</t>
   </si>
   <si>
     <t xml:space="preserve">lancelot</t>
@@ -786,6 +786,9 @@
     <t xml:space="preserve">merlin</t>
   </si>
   <si>
+    <t xml:space="preserve">scenario1.txt(82-87), merlin_log.txt(80-85), merlin_log(88-92), </t>
+  </si>
+  <si>
     <t xml:space="preserve">mordred as ally killer</t>
   </si>
   <si>
@@ -858,10 +861,13 @@
     <t xml:space="preserve">use of Unity or of Spring</t>
   </si>
   <si>
+    <t xml:space="preserve">scenario1.txt(15, 31-38, 43), merlin_log(5, 20-33)</t>
+  </si>
+  <si>
     <t xml:space="preserve">use of JSON</t>
   </si>
   <si>
-    <t xml:space="preserve">equipment_info / quest_setup_cards</t>
+    <t xml:space="preserve">scenario1.txt(76, 85, 103), scenario3.txt(38), merlin_log.txt(90, 95)</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -1013,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D131" activeCellId="0" sqref="D131"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1022,7 +1028,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="94.07"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="5" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.49"/>
   </cols>
@@ -2166,10 +2172,13 @@
       <c r="C112" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D112" s="0" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2178,79 +2187,79 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2259,12 +2268,12 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>146</v>
@@ -2275,7 +2284,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>146</v>
@@ -2286,7 +2295,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>146</v>
@@ -2297,7 +2306,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>146</v>
@@ -2308,7 +2317,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>146</v>
@@ -2319,7 +2328,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>146</v>
@@ -2330,7 +2339,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2339,12 +2348,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2352,10 +2361,13 @@
       <c r="C130" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="D130" s="0" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2364,12 +2376,12 @@
         <v>2</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2378,7 +2390,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grid updates to new logs
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="197">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -657,13 +657,13 @@
     <t xml:space="preserve">   a) correct sponsoring behavior</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log1.txt(74-88, 203-209)</t>
+    <t xml:space="preserve">ai_strategy2_log1.txt(74-88, 203-209), ai_strategy_log2.txt(</t>
   </si>
   <si>
     <t xml:space="preserve">   b) correct behavior for quest participation</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy_log1.txt(94-99, 108-114)</t>
+    <t xml:space="preserve">ai_strategy_log1.txt(94-99, 108-114), ai_strategy_log2.txt(71-75, 98-115)</t>
   </si>
   <si>
     <t xml:space="preserve">   c) correct behavior for tournaments</t>
@@ -675,7 +675,25 @@
     <t xml:space="preserve">   d) correct behavior for bidding</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log1.txt(94-100)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log1.txt(135-163), ai_strategy2_log2.txt(86-98), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log3.txt(111-115)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">is the rule of increasing BPs enforced</t>
@@ -711,7 +729,7 @@
     <t xml:space="preserve">as the game starts, can I select 1 to 3 AI players? (as opposed to always the same # of AIs)</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log2.txt(53-62)</t>
+    <t xml:space="preserve">ai_strategy2_log1.txt(53-62), ai_strategy2_log2.txt(19, 28)</t>
   </si>
   <si>
     <t xml:space="preserve">are discarded cards reusable when A and/or S decks run out</t>
@@ -729,6 +747,9 @@
     <t xml:space="preserve">test of morgan le fey</t>
   </si>
   <si>
+    <t xml:space="preserve">ai_strategy2_log2.txt(53, 86-93)</t>
+  </si>
+  <si>
     <t xml:space="preserve">test of the questing beast</t>
   </si>
   <si>
@@ -796,13 +817,31 @@
     <t xml:space="preserve">lancelot</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log2.txt(114, 125 [Battle points w/ Sir Lancelot])</t>
+    <t xml:space="preserve">ai_strategy2_log2.txt(75, 81 [Battle points w/ Sir Lancelot])</t>
   </si>
   <si>
     <t xml:space="preserve">galahad</t>
   </si>
   <si>
-    <t xml:space="preserve">ai_strategy2_log4.txt(75, 77, 84)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ai_strategy2_log4.txt(75, 77, 84</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Battle points w/ Sir Galahad])</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">merlin</t>
@@ -1054,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D90" activeCellId="0" sqref="D90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2080,34 +2119,37 @@
       <c r="C100" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="D100" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
@@ -2117,7 +2159,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
@@ -2126,7 +2168,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
@@ -2135,7 +2177,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
@@ -2144,7 +2186,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
@@ -2153,7 +2195,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
@@ -2162,55 +2204,55 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
@@ -2219,79 +2261,79 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2300,12 +2342,12 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>146</v>
@@ -2316,7 +2358,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>146</v>
@@ -2327,7 +2369,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>146</v>
@@ -2338,7 +2380,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>146</v>
@@ -2349,7 +2391,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>146</v>
@@ -2360,7 +2402,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>146</v>
@@ -2371,7 +2413,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2380,12 +2422,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2394,12 +2436,12 @@
         <v>15</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2408,12 +2450,12 @@
         <v>2</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2422,12 +2464,12 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to war file
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -675,25 +675,7 @@
     <t xml:space="preserve">   d) correct behavior for bidding</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ai_strategy2_log1.txt(135-163), ai_strategy2_log2.txt(86-98), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ai_strategy2_log3.txt(111-115)</t>
-    </r>
+    <t xml:space="preserve">ai_strategy2_log1.txt(135-163), ai_strategy2_log2.txt(86-98), ai_strategy2_log3.txt(111-115)</t>
   </si>
   <si>
     <t xml:space="preserve">is the rule of increasing BPs enforced</t>
@@ -783,35 +765,7 @@
     <t xml:space="preserve">arthur</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">scenario3.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(48, 54-56</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">) [player only discards 3 due to bonus bids]</t>
-    </r>
+    <t xml:space="preserve">scenario3.txt(48, 54-56) [player only discards 3 due to bonus bids]</t>
   </si>
   <si>
     <t xml:space="preserve">lancelot</t>
@@ -823,25 +777,7 @@
     <t xml:space="preserve">galahad</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ai_strategy2_log4.txt(75, 77, 84</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Battle points w/ Sir Galahad])</t>
-    </r>
+    <t xml:space="preserve">ai_strategy2_log4.txt(75, 77, 84[Battle points w/ Sir Galahad])</t>
   </si>
   <si>
     <t xml:space="preserve">merlin</t>
@@ -928,7 +864,7 @@
     <t xml:space="preserve">use of JSON</t>
   </si>
   <si>
-    <t xml:space="preserve">scenario1.txt(76, 85, 103), scenario3.txt(38), merlin_log.txt(90, 95)</t>
+    <t xml:space="preserve">scenario1.txt(83-86), merlin_log.txt(81-84), merlin_log(88-91)</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -947,7 +883,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -985,12 +921,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1041,7 +971,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,10 +1000,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1093,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D122" activeCellId="0" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1956,7 +1882,7 @@
       <c r="C88" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="5" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2131,7 +2057,7 @@
       <c r="C101" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="5" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2439,7 +2365,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
         <v>192</v>
       </c>
@@ -2449,7 +2375,7 @@
       <c r="C131" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D131" s="0" t="s">
+      <c r="D131" s="5" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up more clean up
</commit_message>
<xml_diff>
--- a/Iteration2-correctionGrid(Web) Version 2.xlsx
+++ b/Iteration2-correctionGrid(Web) Version 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="202">
   <si>
     <t xml:space="preserve">CORRECTION GRID: Iteration 2 for a game running in a browser</t>
   </si>
@@ -723,9 +723,6 @@
     <t xml:space="preserve">do you support a 2-player game</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">test of morgan le fey</t>
   </si>
   <si>
@@ -892,9 +889,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bells and whistles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strategy2 AI Prosperity Event</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1032,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1072,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,8 +2045,8 @@
       <c r="A99" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>146</v>
+      <c r="B99" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -2060,7 +2054,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>21</v>
@@ -2069,12 +2063,12 @@
         <v>0.5</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>21</v>
@@ -2083,124 +2077,124 @@
         <v>0.5</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C109" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C110" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D110" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>21</v>
@@ -2209,12 +2203,12 @@
         <v>0.5</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>21</v>
@@ -2223,108 +2217,108 @@
         <v>2</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="n">
         <v>1.5</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D114" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C114" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D115" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C115" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C116" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D117" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C117" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C118" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D119" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C119" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F120" s="0" t="n">
         <f aca="false">F85+F19+F11</f>
@@ -2333,15 +2327,15 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>146</v>
+        <v>188</v>
+      </c>
+      <c r="B122" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>2</v>
@@ -2349,10 +2343,10 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>146</v>
+        <v>189</v>
+      </c>
+      <c r="B123" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>1</v>
@@ -2360,10 +2354,10 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>146</v>
+        <v>190</v>
+      </c>
+      <c r="B124" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>2</v>
@@ -2371,10 +2365,10 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>146</v>
+        <v>191</v>
+      </c>
+      <c r="B125" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>2</v>
@@ -2382,10 +2376,10 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>146</v>
+        <v>192</v>
+      </c>
+      <c r="B126" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>2</v>
@@ -2393,10 +2387,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>146</v>
+        <v>193</v>
+      </c>
+      <c r="B127" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>2</v>
@@ -2404,7 +2398,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F128" s="0" t="n">
         <f aca="false">F120+SUM(C122:C127)</f>
@@ -2413,12 +2407,12 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>21</v>
@@ -2427,12 +2421,12 @@
         <v>15</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>21</v>
@@ -2441,12 +2435,12 @@
         <v>2</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">SUM(C13:C131)</f>
@@ -2455,12 +2449,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>